<commit_message>
Finalized the project by adding new features
Things added:
-Toggable control buttons
-new Color for toggable buttons
-after a Key is pressed and SHIFT was activated, the mode changes to normal Mode again
-added Label to signalize the user that the window can be moved
-added exit button
</commit_message>
<xml_diff>
--- a/Resources/ButtonData.xlsx
+++ b/Resources/ButtonData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Programmierung\Programme\C#\Standard Implementations\Keyboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Programmierung\Programme\C#\Standard Implementations\On Screen Keyboard\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F89925-82BE-4080-B46C-B7340C088EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5CE7AB-1CA0-447D-A57F-9B92AC27A82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B79870A-B84A-4C57-9F75-1671BB6B8889}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="280">
   <si>
     <t>^</t>
   </si>
@@ -860,6 +860,21 @@
   </si>
   <si>
     <t>RCONTROL</t>
+  </si>
+  <si>
+    <t>altGrShiftMode</t>
+  </si>
+  <si>
+    <t>ẞ</t>
+  </si>
+  <si>
+    <t>Lshift</t>
+  </si>
+  <si>
+    <t>Rshift</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1251,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F1E074-099E-4E9C-8DEF-63C9356E0373}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,10 +1263,11 @@
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>65</v>
       </c>
@@ -1268,13 +1284,16 @@
         <v>210</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
@@ -1290,12 +1309,15 @@
       <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>79</v>
       </c>
@@ -1310,11 +1332,12 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
@@ -1329,11 +1352,12 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -1350,11 +1374,12 @@
         <v>191</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -1371,11 +1396,12 @@
         <v>192</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -1390,11 +1416,12 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
@@ -1409,11 +1436,12 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -1428,11 +1456,12 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -1449,11 +1478,12 @@
         <v>193</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -1470,11 +1500,12 @@
         <v>194</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1491,11 +1522,12 @@
         <v>195</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1512,11 +1544,12 @@
         <v>196</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1532,12 +1565,15 @@
       <c r="E14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
@@ -1548,15 +1584,16 @@
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2</v>
+        <v>279</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>81</v>
       </c>
@@ -1572,14 +1609,17 @@
       <c r="E16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
         <v>98</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -1595,14 +1635,17 @@
       <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
         <v>80</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
@@ -1618,12 +1661,13 @@
       <c r="E18" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -1638,11 +1682,12 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -1659,11 +1704,12 @@
         <v>199</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -1678,11 +1724,12 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>88</v>
       </c>
@@ -1697,11 +1744,12 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -1716,11 +1764,12 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>90</v>
       </c>
@@ -1735,11 +1784,12 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>91</v>
       </c>
@@ -1754,11 +1804,12 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>92</v>
       </c>
@@ -1773,11 +1824,12 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>93</v>
       </c>
@@ -1792,11 +1844,12 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>94</v>
       </c>
@@ -1811,11 +1864,12 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>95</v>
       </c>
@@ -1831,14 +1885,15 @@
       <c r="E29" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
         <v>75</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
@@ -1854,14 +1909,17 @@
       <c r="E30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="1">
         <v>100</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>96</v>
       </c>
@@ -1876,11 +1934,12 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -1895,11 +1954,12 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
@@ -1914,11 +1974,12 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
@@ -1933,11 +1994,12 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
@@ -1952,11 +2014,12 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -1971,11 +2034,12 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>102</v>
       </c>
@@ -1990,11 +2054,12 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
@@ -2009,11 +2074,12 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
@@ -2028,11 +2094,12 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>109</v>
       </c>
@@ -2047,11 +2114,12 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -2066,11 +2134,12 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>111</v>
       </c>
@@ -2085,11 +2154,12 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>107</v>
       </c>
@@ -2105,14 +2175,17 @@
       <c r="E43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G43" s="1">
         <v>80</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -2129,11 +2202,12 @@
         <v>203</v>
       </c>
       <c r="F44" s="1"/>
-      <c r="G44" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>105</v>
       </c>
@@ -2148,11 +2222,12 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>106</v>
       </c>
@@ -2167,11 +2242,12 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -2186,11 +2262,12 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>114</v>
       </c>
@@ -2205,11 +2282,12 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="1"/>
+      <c r="H48" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -2224,11 +2302,12 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="1"/>
+      <c r="H49" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -2243,11 +2322,12 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>117</v>
       </c>
@@ -2264,11 +2344,12 @@
         <v>204</v>
       </c>
       <c r="F51" s="1"/>
-      <c r="G51" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>118</v>
       </c>
@@ -2283,11 +2364,12 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>119</v>
       </c>
@@ -2302,11 +2384,12 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>120</v>
       </c>
@@ -2321,11 +2404,12 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>122</v>
       </c>
@@ -2341,14 +2425,17 @@
       <c r="E55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G55" s="1">
         <v>73</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>123</v>
       </c>
@@ -2364,12 +2451,15 @@
       <c r="E56" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>143</v>
       </c>
@@ -2385,12 +2475,15 @@
       <c r="E57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
@@ -2406,12 +2499,15 @@
       <c r="E58" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1" t="s">
+      <c r="F58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>125</v>
       </c>
@@ -2427,12 +2523,15 @@
       <c r="E59" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1" t="s">
+      <c r="F59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>126</v>
       </c>
@@ -2448,12 +2547,15 @@
       <c r="E60" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1" t="s">
+      <c r="F60" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>127</v>
       </c>
@@ -2469,12 +2571,15 @@
       <c r="E61" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1" t="s">
+      <c r="F61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>128</v>
       </c>
@@ -2484,14 +2589,15 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1">
         <v>393</v>
       </c>
-      <c r="G62" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
@@ -2507,12 +2613,15 @@
       <c r="E63" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
+      <c r="F63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
@@ -2528,12 +2637,15 @@
       <c r="E64" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1" t="s">
+      <c r="F64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
@@ -2549,12 +2661,15 @@
       <c r="E65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>132</v>
       </c>
@@ -2570,12 +2685,15 @@
       <c r="E66" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
@@ -2591,12 +2709,15 @@
       <c r="E67" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
@@ -2612,12 +2733,15 @@
       <c r="E68" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>135</v>
       </c>
@@ -2633,12 +2757,15 @@
       <c r="E69" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F69" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
@@ -2654,12 +2781,15 @@
       <c r="E70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F70" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>137</v>
       </c>
@@ -2675,12 +2805,15 @@
       <c r="E71" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F71" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -2696,12 +2829,15 @@
       <c r="E72" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F72" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>139</v>
       </c>
@@ -2717,12 +2853,15 @@
       <c r="E73" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>140</v>
       </c>
@@ -2738,12 +2877,15 @@
       <c r="E74" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F74" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>141</v>
       </c>
@@ -2759,12 +2901,15 @@
       <c r="E75" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>142</v>
       </c>
@@ -2780,12 +2925,15 @@
       <c r="E76" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F76" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>144</v>
       </c>
@@ -2801,12 +2949,15 @@
       <c r="E77" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F77" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>145</v>
       </c>
@@ -2822,12 +2973,15 @@
       <c r="E78" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F78" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>146</v>
       </c>
@@ -2843,8 +2997,11 @@
       <c r="E79" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1" t="s">
+      <c r="F79" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>